<commit_message>
post amendments, update readme.
</commit_message>
<xml_diff>
--- a/Attachment C-1 Technical Qualifications amended.xlsx
+++ b/Attachment C-1 Technical Qualifications amended.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="991" documentId="8_{B9EE35BC-2C34-439D-BBE0-BD6628FB0B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7B8F1A9-92AD-4F2E-BBE1-B1B93D0CD56C}"/>
+  <xr:revisionPtr revIDLastSave="1007" documentId="8_{B9EE35BC-2C34-439D-BBE0-BD6628FB0B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3613AC1D-0BAC-4439-8D74-09644BC0CE05}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="665" xr2:uid="{8A1DC20E-A95C-431F-90C4-822735B01E86}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="665" activeTab="2" xr2:uid="{8A1DC20E-A95C-431F-90C4-822735B01E86}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="15" r:id="rId1"/>
@@ -508,16 +508,17 @@
     <t>All resumes submitted by the offeror are for current or recent (within 1 year) employees or are also accompanied by commitment letters.</t>
   </si>
   <si>
-    <t>All resumes submitted by the offeror demonstrate that the proposed FTE meets or exceeds the minimum years of relevant experience(s) listed under "Required Experience", has at least one of the certification(s) listed under "Certifications" and has experience with at least one of the key technologies/software listed under "Skills and Qualifications" for the CLIN in Section H.3 of the RFQ document.</t>
-  </si>
-  <si>
     <t>The offeror will provide a High-Risk Public Trust (Tier 4) background check for all staff augmentees assigned to the contract. Contractor personnel may start working at the Court on a provisional basis for up to 1 year with a Tier 1 background check while the Tier 4 background check is being processed. Use of a qualified third-party service for processing the Tier 4 high risk public trust (HRPT) or equivalent background check is allowed.</t>
   </si>
   <si>
-    <t>The offeror shall provide a qualified replacement for Court approval within 5 business days of any unplanned personnel departure (e.g. sudden unforeseen termination) and 5 business days before any planned departure (e.g. resignation with notice) to ensure relatively continuous coverage of the position. The replacement must meet or exceed the qualifications of the original personnel and must start work no later than 20 business days after receiving Court approval.</t>
-  </si>
-  <si>
-    <t>The offeror shall notify the Court at least 10 business days before any position will have a temporary vacancy (e.g. PTO or any other leave) longer than 5 business days, and provide a qualified temporary substitute for the duration of the planned vacancy beyond the initial 5 days. The replacement must meet or exceed the qualifications of the original personnel.</t>
+    <t>All resumes submitted by the offeror demonstrate that the proposed FTE meets or exceeds the minimum years of relevant experience(s) listed under "Required Experience", has at least one of the certification(s) listed under "Certifications" and has experience with at least one of the key technologies/software listed under "Skills and Qualifications" for the CLIN in Section H.3 of the RFQ document.
+Certifications should be acquired before the RFQ close date. Only in cases where the certification doesn't have opportunities to acquire before the closing of the RFQ, the Court will consider an in-progress certification technically acceptable if the offeror provides a paid-for schedule/receipt showing the exam date.</t>
+  </si>
+  <si>
+    <t>The offeror shall notify the Court at least 10 business days before any position will have a temporary vacancy (e.g. PTO or any other leave) longer than 5 business days, and provide a qualified temporary substitute for the duration of the planned vacancy beyond the initial 5 days. The replacement must meet or exceed the qualifications of the original personnel. In the event of any discrepancy between this requirement and Clause 2-65, this requirement shall take precedence.</t>
+  </si>
+  <si>
+    <t>The offeror shall provide a qualified replacement for Court approval within 5 business days of any unplanned personnel departure (e.g. sudden unforeseen termination) and 5 business days before any planned departure (e.g. resignation with notice) to ensure relatively continuous coverage of the position. The replacement must meet or exceed the qualifications of the original personnel and must start work no later than 20 business days after receiving Court approval. In the event of any discrepancy between this requirement and Clause 2-65, this requirement shall take precedence.</t>
   </si>
 </sst>
 </file>
@@ -1594,7 +1595,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
@@ -1619,7 +1620,7 @@
   <cols>
     <col min="1" max="1" width="8.88671875" style="8"/>
     <col min="2" max="2" width="12" style="8" customWidth="1"/>
-    <col min="3" max="3" width="89.77734375" style="10" customWidth="1"/>
+    <col min="3" max="3" width="89.6640625" style="10" customWidth="1"/>
     <col min="4" max="5" width="8.88671875" style="8"/>
     <col min="6" max="6" width="12.109375" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="8.88671875" style="8"/>
@@ -1890,7 +1891,7 @@
   </sheetPr>
   <dimension ref="B1:F31"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -1898,7 +1899,7 @@
   <cols>
     <col min="1" max="1" width="8.88671875" style="8"/>
     <col min="2" max="2" width="13.109375" style="8" customWidth="1"/>
-    <col min="3" max="3" width="72.21875" style="10" customWidth="1"/>
+    <col min="3" max="3" width="72.33203125" style="10" customWidth="1"/>
     <col min="4" max="4" width="8.88671875" style="8"/>
     <col min="5" max="5" width="12.6640625" style="8" customWidth="1"/>
     <col min="6" max="6" width="37.88671875" style="8" customWidth="1"/>
@@ -2031,12 +2032,12 @@
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="2:6" ht="109.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" ht="125.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>3</v>
@@ -2044,12 +2045,12 @@
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="2:6" ht="78.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" ht="109.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>3</v>
@@ -2088,7 +2089,7 @@
         <v>75</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>3</v>
@@ -2252,12 +2253,12 @@
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
     </row>
-    <row r="30" spans="2:6" ht="94.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" ht="179.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="1" t="s">
         <v>125</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>3</v>
@@ -2302,7 +2303,7 @@
   <dimension ref="B1:F14"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2311,7 +2312,7 @@
     <col min="2" max="2" width="15.88671875" style="8" customWidth="1"/>
     <col min="3" max="3" width="72" style="8" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="8" customWidth="1"/>
     <col min="6" max="6" width="46.6640625" style="8" customWidth="1"/>
     <col min="7" max="16384" width="8.88671875" style="8"/>
   </cols>
@@ -2378,7 +2379,7 @@
       </c>
     </row>
     <row r="8" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="2:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="11" t="s">
         <v>126</v>
       </c>
@@ -2491,9 +2492,9 @@
     <col min="1" max="1" width="8.88671875" style="8"/>
     <col min="2" max="2" width="14.5546875" style="8" customWidth="1"/>
     <col min="3" max="3" width="67.6640625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="9.21875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="8" customWidth="1"/>
     <col min="5" max="5" width="13.109375" style="8" customWidth="1"/>
-    <col min="6" max="6" width="38.21875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="38.33203125" style="8" customWidth="1"/>
     <col min="7" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
@@ -2559,7 +2560,7 @@
       </c>
     </row>
     <row r="8" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="2:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="11" t="s">
         <v>126</v>
       </c>
@@ -2726,19 +2727,19 @@
   </sheetPr>
   <dimension ref="B1:F16"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" style="8"/>
+    <col min="1" max="1" width="8.6640625" style="8"/>
     <col min="2" max="2" width="12.44140625" style="8" customWidth="1"/>
     <col min="3" max="3" width="57.88671875" style="8" customWidth="1"/>
     <col min="4" max="4" width="10.109375" style="8" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" style="8" customWidth="1"/>
     <col min="6" max="6" width="45.44140625" style="8" customWidth="1"/>
-    <col min="7" max="16384" width="8.77734375" style="8"/>
+    <col min="7" max="16384" width="8.6640625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -2940,7 +2941,7 @@
   </sheetPr>
   <dimension ref="B1:F19"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -3275,7 +3276,7 @@
       </c>
     </row>
     <row r="8" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="2:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="13" t="s">
         <v>126</v>
       </c>

</xml_diff>